<commit_message>
add new changes in relation to multiple clients in managing of LA states
</commit_message>
<xml_diff>
--- a/STS IR Bot Performer/Data/Output/SC ST 389 tool YOUNIQUE.xlsx
+++ b/STS IR Bot Performer/Data/Output/SC ST 389 tool YOUNIQUE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\martin.martinez\Documents\github-IRBot\STS_InternalReviewBot\STS IR Bot Performer\Data\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{055E8089-7608-4B52-B2CE-3B9A1A762488}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14E4FF2D-C05D-467C-834B-A0D00E7B402F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1815" yWindow="1815" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2160" yWindow="2160" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SC ST-389 tool" sheetId="1" r:id="rId1"/>

</xml_diff>